<commit_message>
change date format to YYYY-MM-DDThh:mm:ssZ
</commit_message>
<xml_diff>
--- a/chl-transect-underway-discrete.xlsx
+++ b/chl-transect-underway-discrete.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20380"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20382"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sbeaulieu\Desktop\github\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jfutrelle\Documents\GitHub\nes-lter-chl-transect-underway-discrete\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CAFA3B2-8989-45B6-8650-C4C539B9654C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86FFFA62-15B3-42A1-8583-25C226D21CF8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="18060" windowHeight="9756" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -81,9 +81,6 @@
     <t>categorical</t>
   </si>
   <si>
-    <t>YYYY-MM-DD hh:mm:ss</t>
-  </si>
-  <si>
     <t>degree</t>
   </si>
   <si>
@@ -136,13 +133,16 @@
   </si>
   <si>
     <t>Depth of underway seawater intake below sea surface</t>
+  </si>
+  <si>
+    <t>YYYY-MM-DDThh:mm:ssZ</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -156,6 +156,11 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial Unicode MS"/>
     </font>
   </fonts>
   <fills count="2">
@@ -178,12 +183,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -501,17 +509,17 @@
   <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
   <cols>
     <col min="1" max="1" width="26.19921875" customWidth="1"/>
     <col min="2" max="2" width="65" customWidth="1"/>
-    <col min="5" max="5" width="20.3984375" customWidth="1"/>
+    <col min="5" max="5" width="23.59765625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -534,165 +542,165 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7">
       <c r="A2" t="s">
         <v>7</v>
       </c>
       <c r="B2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C2" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7">
       <c r="A3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C3" t="s">
         <v>15</v>
       </c>
-      <c r="E3" t="s">
-        <v>18</v>
+      <c r="E3" s="3" t="s">
+        <v>36</v>
       </c>
       <c r="F3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G3" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
       <c r="A4" t="s">
         <v>11</v>
       </c>
       <c r="B4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C4" t="s">
         <v>16</v>
       </c>
       <c r="D4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G4" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
       <c r="A5" t="s">
         <v>12</v>
       </c>
       <c r="B5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C5" t="s">
         <v>16</v>
       </c>
       <c r="D5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G5" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
       <c r="A6" t="s">
         <v>13</v>
       </c>
       <c r="B6" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C6" t="s">
         <v>16</v>
       </c>
       <c r="D6" t="s">
+        <v>19</v>
+      </c>
+      <c r="F6" t="s">
+        <v>26</v>
+      </c>
+      <c r="G6" t="s">
         <v>20</v>
       </c>
-      <c r="F6" t="s">
-        <v>27</v>
-      </c>
-      <c r="G6" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="7" spans="1:7">
       <c r="A7" t="s">
         <v>8</v>
       </c>
       <c r="B7" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C7" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7">
       <c r="A8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C8" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7">
       <c r="A9" t="s">
         <v>9</v>
       </c>
       <c r="B9" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>16</v>
       </c>
       <c r="D9" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F9" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G9" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7">
       <c r="A10" t="s">
         <v>10</v>
       </c>
       <c r="B10" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>16</v>
       </c>
       <c r="D10" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F10" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G10" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7">
       <c r="A11" t="s">
+        <v>28</v>
+      </c>
+      <c r="B11" t="s">
         <v>29</v>
-      </c>
-      <c r="B11" t="s">
-        <v>30</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>17</v>
@@ -700,5 +708,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>